<commit_message>
changed 25-1 to NA since it isn't a usable sample
</commit_message>
<xml_diff>
--- a/data/new_carcass_site_data.xlsx
+++ b/data/new_carcass_site_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billy.DESKTOP-6FIO124\Documents\MS\Food For The Masses\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billy.DESKTOP-6FIO124\Documents\Master Thesis\food_for_the_masses\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429DB98A-B9BE-4EE0-96AB-B4E2203FDE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B6BDDE-F95E-4F59-A6D1-8D6FF46F027B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="334">
   <si>
     <t>Kill .</t>
   </si>
@@ -1022,6 +1022,9 @@
   </si>
   <si>
     <t>25-088</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1040,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1056,6 +1059,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1069,7 +1078,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1077,6 +1086,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1384,8 +1394,8 @@
   <dimension ref="A1:AE100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7051,6 +7061,9 @@
       </c>
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A71" s="5" t="s">
+        <v>333</v>
+      </c>
       <c r="B71" t="s">
         <v>218</v>
       </c>

</xml_diff>

<commit_message>
fixed previously unentered cougar kill (23-051 -> 23-292)
</commit_message>
<xml_diff>
--- a/data/new_carcass_site_data.xlsx
+++ b/data/new_carcass_site_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billy.DESKTOP-6FIO124\Documents\Master Thesis\food_for_the_masses\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B6BDDE-F95E-4F59-A6D1-8D6FF46F027B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADE6758-AA81-4917-AE0E-C7BFED06CFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -922,9 +922,6 @@
     <t>23-030</t>
   </si>
   <si>
-    <t>23-051</t>
-  </si>
-  <si>
     <t>23-064</t>
   </si>
   <si>
@@ -1025,6 +1022,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>23-292</t>
   </si>
 </sst>
 </file>
@@ -1394,8 +1394,8 @@
   <dimension ref="A1:AE100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7062,7 +7062,7 @@
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B71" t="s">
         <v>218</v>
@@ -7335,7 +7335,7 @@
         <v>282</v>
       </c>
       <c r="E74" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F74">
         <v>546890</v>
@@ -8367,7 +8367,7 @@
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
-        <v>299</v>
+        <v>333</v>
       </c>
       <c r="B86" t="s">
         <v>218</v>
@@ -8450,7 +8450,7 @@
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B87" t="s">
         <v>218</v>
@@ -8536,7 +8536,7 @@
     </row>
     <row r="88" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B88" t="s">
         <v>218</v>
@@ -8548,7 +8548,7 @@
         <v>226</v>
       </c>
       <c r="E88" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F88">
         <v>534681</v>
@@ -8625,7 +8625,7 @@
     </row>
     <row r="89" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B89" t="s">
         <v>218</v>
@@ -8637,7 +8637,7 @@
         <v>226</v>
       </c>
       <c r="E89" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F89">
         <v>535464</v>
@@ -8705,7 +8705,7 @@
     </row>
     <row r="90" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B90" t="s">
         <v>218</v>
@@ -8783,7 +8783,7 @@
         <v>1</v>
       </c>
       <c r="AC90" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AD90">
         <v>0</v>
@@ -8794,7 +8794,7 @@
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B91" t="s">
         <v>218</v>
@@ -8806,7 +8806,7 @@
         <v>208</v>
       </c>
       <c r="E91" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F91">
         <v>546209</v>
@@ -8866,7 +8866,7 @@
         <v>2</v>
       </c>
       <c r="AC91" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AD91">
         <v>0</v>
@@ -8877,7 +8877,7 @@
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B92" t="s">
         <v>218</v>
@@ -8889,7 +8889,7 @@
         <v>208</v>
       </c>
       <c r="E92" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F92">
         <v>553188</v>
@@ -8952,7 +8952,7 @@
         <v>5</v>
       </c>
       <c r="AC92" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AD92">
         <v>0</v>
@@ -8963,7 +8963,7 @@
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B93" t="s">
         <v>218</v>
@@ -8972,7 +8972,7 @@
         <v>45360</v>
       </c>
       <c r="D93" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E93" t="s">
         <v>33</v>
@@ -8987,7 +8987,7 @@
         <v>45357</v>
       </c>
       <c r="I93" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J93" t="s">
         <v>42</v>
@@ -9046,7 +9046,7 @@
     </row>
     <row r="94" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B94" t="s">
         <v>218</v>
@@ -9058,7 +9058,7 @@
         <v>226</v>
       </c>
       <c r="E94" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F94">
         <v>545857</v>
@@ -9121,7 +9121,7 @@
         <v>0</v>
       </c>
       <c r="AC94" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AD94">
         <v>0</v>
@@ -9132,7 +9132,7 @@
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B95" t="s">
         <v>218</v>
@@ -9144,7 +9144,7 @@
         <v>226</v>
       </c>
       <c r="E95" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F95">
         <v>547780</v>
@@ -9215,7 +9215,7 @@
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B96" t="s">
         <v>218</v>
@@ -9290,7 +9290,7 @@
         <v>5</v>
       </c>
       <c r="AC96" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD96">
         <v>0</v>
@@ -9301,7 +9301,7 @@
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B97" t="s">
         <v>218</v>
@@ -9313,7 +9313,7 @@
         <v>282</v>
       </c>
       <c r="E97" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F97">
         <v>543022</v>
@@ -9325,7 +9325,7 @@
         <v>45626</v>
       </c>
       <c r="I97" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J97" t="s">
         <v>37</v>
@@ -9376,7 +9376,7 @@
         <v>0</v>
       </c>
       <c r="AC97" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AD97">
         <v>0</v>
@@ -9387,7 +9387,7 @@
     </row>
     <row r="98" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B98" t="s">
         <v>218</v>
@@ -9399,7 +9399,7 @@
         <v>226</v>
       </c>
       <c r="E98" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H98" s="2">
         <v>45638</v>
@@ -9464,7 +9464,7 @@
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B99" t="s">
         <v>218</v>
@@ -9473,7 +9473,7 @@
         <v>45727</v>
       </c>
       <c r="D99" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E99" t="s">
         <v>294</v>
@@ -9530,7 +9530,7 @@
         <v>5</v>
       </c>
       <c r="AC99" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AD99">
         <v>0</v>
@@ -9541,7 +9541,7 @@
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B100" t="s">
         <v>218</v>
@@ -9607,7 +9607,7 @@
         <v>0</v>
       </c>
       <c r="AC100" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AD100">
         <v>0</v>

</xml_diff>

<commit_message>
added species data for 22-115 (adult cow elk)
</commit_message>
<xml_diff>
--- a/data/new_carcass_site_data.xlsx
+++ b/data/new_carcass_site_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billy.DESKTOP-6FIO124\Documents\Master Thesis\food_for_the_masses\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAD7AA5-25A5-42EF-A0DC-B6A3CC3EB605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7235D0B-C754-4D4A-9C94-605C2365D738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="334">
   <si>
     <t>Kill .</t>
   </si>
@@ -1393,9 +1393,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V68" sqref="V68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7174,6 +7174,9 @@
       <c r="I72" t="s">
         <v>35</v>
       </c>
+      <c r="J72" t="s">
+        <v>42</v>
+      </c>
       <c r="K72" t="s">
         <v>59</v>
       </c>

</xml_diff>